<commit_message>
fix template for 0.3 with relative and absolute paths
</commit_message>
<xml_diff>
--- a/projects/office_ideal_calibration.xlsx
+++ b/projects/office_ideal_calibration.xlsx
@@ -2452,25 +2452,25 @@
     <t>../lib/calibration_data</t>
   </si>
   <si>
+    <t>Path (relative to this spreadsheet or absolute path)</t>
+  </si>
+  <si>
+    <t>Relative to this spreadsheet or absolute path</t>
+  </si>
+  <si>
+    <t>Weather Directory</t>
+  </si>
+  <si>
+    <t>weather_directory</t>
+  </si>
+  <si>
+    <t>../../weather</t>
+  </si>
+  <si>
+    <t>office_calibration</t>
+  </si>
+  <si>
     <t>Files to include (relative to this spreadsheet or absolute path). If a directory then it will include all subfolders and files</t>
-  </si>
-  <si>
-    <t>Path (relative to this spreadsheet or absolute path)</t>
-  </si>
-  <si>
-    <t>Relative to this spreadsheet or absolute path</t>
-  </si>
-  <si>
-    <t>Weather Directory</t>
-  </si>
-  <si>
-    <t>weather_directory</t>
-  </si>
-  <si>
-    <t>../../weather</t>
-  </si>
-  <si>
-    <t>office_calibration</t>
   </si>
 </sst>
 </file>
@@ -2605,7 +2605,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1758">
+  <cellStyleXfs count="1774">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4356,6 +4356,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4455,7 +4471,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1758">
+  <cellStyles count="1774">
     <cellStyle name="Comma" xfId="1749" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -5335,6 +5351,14 @@
     <cellStyle name="Followed Hyperlink" xfId="1753" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1755" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1757" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1759" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1761" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1763" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1765" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1767" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1769" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1771" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1773" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6213,6 +6237,14 @@
     <cellStyle name="Hyperlink" xfId="1752" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1754" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1756" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1758" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1760" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1762" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1764" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1766" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1768" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1770" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1772" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6548,8 +6580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6703,7 +6735,7 @@
         <v>696</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -6714,7 +6746,7 @@
         <v>695</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -6868,7 +6900,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>31</v>
@@ -6895,7 +6927,7 @@
         <v>38</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>449</v>
@@ -6906,7 +6938,7 @@
         <v>32</v>
       </c>
       <c r="B40" s="31" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="C40" s="31" t="s">
         <v>680</v>
@@ -6926,7 +6958,7 @@
         <v>34</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>803</v>
+        <v>809</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="13" t="s">
@@ -7153,16 +7185,16 @@
         <v>21</v>
       </c>
       <c r="D5" s="30" t="s">
+        <v>805</v>
+      </c>
+      <c r="E5" s="30" t="s">
         <v>806</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>807</v>
       </c>
       <c r="F5" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="6" spans="1:25" s="30" customFormat="1">

</xml_diff>

<commit_message>
remove name of building so that it creates a uuid
</commit_message>
<xml_diff>
--- a/projects/office_ideal_calibration.xlsx
+++ b/projects/office_ideal_calibration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16840" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20440" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2376" uniqueCount="810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2375" uniqueCount="809">
   <si>
     <t>type</t>
   </si>
@@ -2465,9 +2465,6 @@
   </si>
   <si>
     <t>../../weather</t>
-  </si>
-  <si>
-    <t>office_calibration</t>
   </si>
   <si>
     <t>Files to include (relative to this spreadsheet or absolute path). If a directory then it will include all subfolders and files</t>
@@ -6580,8 +6577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6937,9 +6934,6 @@
       <c r="A40" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="31" t="s">
-        <v>808</v>
-      </c>
       <c r="C40" s="31" t="s">
         <v>680</v>
       </c>
@@ -6958,7 +6952,7 @@
         <v>34</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="13" t="s">
@@ -7007,8 +7001,8 @@
   <dimension ref="A1:Y222"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <pane ySplit="3" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>